<commit_message>
start paper v1 8/5
</commit_message>
<xml_diff>
--- a/code/documentation.xlsx
+++ b/code/documentation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,15 +46,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>However, for Slovenia the numbers from ISIC3 are way larger than those from ISIC4. I suspect in ISIC3 the units are millions of Slovenian tolar while in ISIC4 the units are millions of Euros. However, after converting the ISIC3 numbers by the Euro fixed rates, there is still some big discrepancy.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Combine data on total outward MNE activities in AMNE_OUT4_world_tot_fin.dta into activity_out.dta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Germany's monetary values in 2007 is about 1000 times larger than previous years. Adjusted back to make the time series consistent.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -182,10 +174,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Exchange rates adjustments: for countries that haven't joined Euro Zone, use WDI exchange rates; for countries that are in the Euro Zone, use Euro exchange rates after year of adoption. For Euro Zone countries before year of adoption, first use the fixed rate to translate the numbers into LCU and then use the WDI exchange rates to translate into USD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>eurostat_ind_agg.do</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,6 +199,59 @@
   </si>
   <si>
     <t>Drop cases where home country is the same as host country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust for exchange rates. Mil of EUR/ECU to USD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oecd_ind_agg.do</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>combine OECD MNE activities, FDI flows and stocks data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust for outliers: Germany in 2007 (isic3), Slovenia for all years (isic3) 1000 times smaller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adjust for exchange rates. Mil of LCU to USD.For countries that haven't joined Euro Zone, use WDI exchange rates; for countries that are in the Euro Zone, use Euro exchange rates after year of adoption. For Euro Zone countries before year of adoption, first use the fixed rate to translate the numbers into LCU and then use the WDI exchange rates to translate into USD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>consolidate_emp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>consolidate two employment variables, n_emp and n_psn_emp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use n_psn_emp as primary data and supplement with n_emp. Produce corresponding comparison tables for OECD inward/outward, and Eurostat inward.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extrap_bilat_activities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>drop time series anomalies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supplement missing country in Eurostat with OECD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Filling missing values: (1) use the corresponding variable from the other data source (OECD - ES or ES - OECD)
+(2) impute zero if non-positive FDI stock
+(3) impute zero revenue if zero employment or zero # enterprise (at least one)
+(4) impute zero revenue if all records (emp,ent,rev) of the opposite direction are zero (or missing, at least one zero)
+(5) use 
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -590,10 +631,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -603,36 +644,45 @@
     </row>
     <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="81" x14ac:dyDescent="0.15">
-      <c r="D5" s="1" t="s">
+    <row r="7" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="D7" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="D7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="81" x14ac:dyDescent="0.15">
@@ -640,10 +690,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -653,43 +703,67 @@
     </row>
     <row r="10" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="121.5" x14ac:dyDescent="0.15">
+      <c r="D19" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>